<commit_message>
ajuste de ordem e filtro
</commit_message>
<xml_diff>
--- a/dados/kaique/dados.xlsx
+++ b/dados/kaique/dados.xlsx
@@ -467,26 +467,26 @@
     </row>
     <row r="2">
       <c r="A2" t="n">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Patos</t>
+          <t>Texeira</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>01/05/2024</t>
+          <t>02/05/2024</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>24/05/2024</t>
+          <t>31/05/2024</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>nacional</t>
+          <t>internacional</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -497,21 +497,21 @@
     </row>
     <row r="3">
       <c r="A3" t="n">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>teixeira</t>
+          <t>patos</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>01/05/2024</t>
+          <t>02/05/2024</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>30/05/2024</t>
+          <t>31/05/2024</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -521,7 +521,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>trabalho</t>
+          <t>lazer</t>
         </is>
       </c>
     </row>

</xml_diff>